<commit_message>
Update GOA dusky rockfish
</commit_message>
<xml_diff>
--- a/examples/Species_Specific_Case_Studies/Test_GOA_Dusky_rockfish/Bias Correction Comparison.xlsx
+++ b/examples/Species_Specific_Case_Studies/Test_GOA_Dusky_rockfish/Bias Correction Comparison.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curryc2/Documents/NOAA/2017/VAST Evaluation/AFSC_VAST_Evaluation/examples/Species_Specific_Case_Studies/Test_GOA_Dusky_rockfish/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FADC713-77A1-C64D-BB17-252AF2A900CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16460" yWindow="700" windowWidth="25040" windowHeight="17820" tabRatio="500"/>
+    <workbookView xWindow="8380" yWindow="440" windowWidth="25040" windowHeight="17820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,8 +36,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -42,6 +48,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -68,9 +81,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -78,6 +92,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -402,16 +424,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,8 +443,14 @@
       <c r="C1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -432,8 +460,14 @@
       <c r="C2">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>1000</v>
+      </c>
+      <c r="I2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>1984</v>
       </c>
@@ -451,8 +485,18 @@
         <f>D3/C3</f>
         <v>-5.5644999488655734E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <v>20664.4344417381</v>
+      </c>
+      <c r="G3" s="1">
+        <f>(F3-B3)/B3</f>
+        <v>-0.10400351968322902</v>
+      </c>
+      <c r="I3" s="2">
+        <v>23367.395100000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>1985</v>
       </c>
@@ -470,8 +514,18 @@
         <f t="shared" ref="E4:E36" si="1">D4/C4</f>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" ref="G4:G38" si="2">(F4-B4)/B4</f>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I4" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>1986</v>
       </c>
@@ -489,8 +543,18 @@
         <f t="shared" si="1"/>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I5" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>1987</v>
       </c>
@@ -508,8 +572,18 @@
         <f t="shared" si="1"/>
         <v>-5.1480555216730318E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <v>35737.516735552097</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.1680152839756377</v>
+      </c>
+      <c r="I6" s="2">
+        <v>40961.971100000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>1988</v>
       </c>
@@ -527,8 +601,18 @@
         <f t="shared" si="1"/>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I7" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>1989</v>
       </c>
@@ -546,8 +630,18 @@
         <f t="shared" si="1"/>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I8" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>1990</v>
       </c>
@@ -565,8 +659,18 @@
         <f t="shared" si="1"/>
         <v>-6.036316234442702E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9">
+        <v>23366.18921461</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.14676829902023067</v>
+      </c>
+      <c r="I9" s="2">
+        <v>27908.393</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>1991</v>
       </c>
@@ -584,8 +688,18 @@
         <f t="shared" si="1"/>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I10" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>1992</v>
       </c>
@@ -603,8 +717,18 @@
         <f t="shared" si="1"/>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I11" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>1993</v>
       </c>
@@ -622,8 +746,18 @@
         <f t="shared" si="1"/>
         <v>-5.8819749482669589E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12">
+        <v>32124.372571352</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.10871654335324567</v>
+      </c>
+      <c r="I12" s="2">
+        <v>36561.230799999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>1994</v>
       </c>
@@ -641,8 +775,18 @@
         <f t="shared" si="1"/>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I13" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>1995</v>
       </c>
@@ -660,8 +804,18 @@
         <f t="shared" si="1"/>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I14" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>1996</v>
       </c>
@@ -679,8 +833,18 @@
         <f t="shared" si="1"/>
         <v>-6.2391455842251947E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15">
+        <v>32871.570901314597</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.11572243350841568</v>
+      </c>
+      <c r="I15" s="2">
+        <v>37688.863700000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>1997</v>
       </c>
@@ -698,8 +862,18 @@
         <f t="shared" si="1"/>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I16" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>1998</v>
       </c>
@@ -717,8 +891,18 @@
         <f t="shared" si="1"/>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I17" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>1999</v>
       </c>
@@ -736,8 +920,18 @@
         <f t="shared" si="1"/>
         <v>-6.3209765603549573E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18">
+        <v>30761.558114880001</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="2"/>
+        <v>-3.0134530949180127E-2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>36031.722099999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>2000</v>
       </c>
@@ -755,8 +949,18 @@
         <f t="shared" si="1"/>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I19" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>2001</v>
       </c>
@@ -774,8 +978,18 @@
         <f t="shared" si="1"/>
         <v>-6.7433382912861536E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20">
+        <v>39919.313958904197</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.1015677975111012</v>
+      </c>
+      <c r="I20" s="2">
+        <v>45993.1734</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>2002</v>
       </c>
@@ -793,8 +1007,18 @@
         <f t="shared" si="1"/>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I21" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>2003</v>
       </c>
@@ -812,8 +1036,18 @@
         <f t="shared" si="1"/>
         <v>-6.0416784896885685E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22">
+        <v>45065.064646496998</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="2"/>
+        <v>-3.2604689620420152E-2</v>
+      </c>
+      <c r="I22" s="2">
+        <v>50680.900900000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>2004</v>
       </c>
@@ -831,8 +1065,18 @@
         <f t="shared" si="1"/>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I23" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>2005</v>
       </c>
@@ -850,8 +1094,18 @@
         <f t="shared" si="1"/>
         <v>-5.5557744965905161E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24">
+        <v>66401.077111669903</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="2"/>
+        <v>-3.9730137048678983E-2</v>
+      </c>
+      <c r="I24" s="2">
+        <v>76310.994699999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>2006</v>
       </c>
@@ -869,8 +1123,18 @@
         <f t="shared" si="1"/>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I25" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>2007</v>
       </c>
@@ -888,8 +1152,18 @@
         <f t="shared" si="1"/>
         <v>-5.7864065650526847E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26">
+        <v>42677.3287126539</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.11949903501600362</v>
+      </c>
+      <c r="I26" s="2">
+        <v>50655.8537</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>2008</v>
       </c>
@@ -907,8 +1181,18 @@
         <f t="shared" si="1"/>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I27" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>2009</v>
       </c>
@@ -926,8 +1210,18 @@
         <f t="shared" si="1"/>
         <v>-6.0086653450252943E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28">
+        <v>33858.708918258097</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.17512642493712802</v>
+      </c>
+      <c r="I28" s="2">
+        <v>42053.387799999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>2010</v>
       </c>
@@ -945,8 +1239,18 @@
         <f t="shared" si="1"/>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I29" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>2011</v>
       </c>
@@ -964,8 +1268,18 @@
         <f t="shared" si="1"/>
         <v>-6.1912069027860311E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30">
+        <v>38096.061743264501</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="2"/>
+        <v>-9.2459643834346558E-2</v>
+      </c>
+      <c r="I30" s="2">
+        <v>44506.561399999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>2012</v>
       </c>
@@ -983,8 +1297,18 @@
         <f t="shared" si="1"/>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I31" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>2013</v>
       </c>
@@ -1002,8 +1326,18 @@
         <f t="shared" si="1"/>
         <v>-6.0415668352465632E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32">
+        <v>54122.789507218004</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.12735096770026846</v>
+      </c>
+      <c r="I32" s="2">
+        <v>62920.113700000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>2014</v>
       </c>
@@ -1021,8 +1355,18 @@
         <f t="shared" si="1"/>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I33" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>2015</v>
       </c>
@@ -1040,8 +1384,18 @@
         <f t="shared" si="1"/>
         <v>-5.7719772711264078E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34">
+        <v>51720.603829539403</v>
+      </c>
+      <c r="G34" s="1">
+        <f t="shared" si="2"/>
+        <v>-8.5157413619496872E-2</v>
+      </c>
+      <c r="I34" s="2">
+        <v>61673.542099999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>2016</v>
       </c>
@@ -1059,8 +1413,18 @@
         <f t="shared" si="1"/>
         <v>-0.11382761757026927</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G35" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5431700234127512</v>
+      </c>
+      <c r="I35" s="2">
+        <v>3596.5447600000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>2017</v>
       </c>
@@ -1078,8 +1442,54 @@
         <f t="shared" si="1"/>
         <v>-5.8654805665813645E-2</v>
       </c>
+      <c r="F36">
+        <v>54009.065391914199</v>
+      </c>
+      <c r="G36" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.23280134235776789</v>
+      </c>
+      <c r="I36" s="2">
+        <v>66091.195800000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37">
+        <v>2018</v>
+      </c>
+      <c r="F37">
+        <v>4132.5273400495598</v>
+      </c>
+      <c r="G37" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38">
+        <v>2019</v>
+      </c>
+      <c r="F38">
+        <v>76444.733795847802</v>
+      </c>
+      <c r="G38" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G3:G36">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>